<commit_message>
update dict example 62
</commit_message>
<xml_diff>
--- a/Examples/Dictionary/Input/Exp62_RatingsSetup_empty.xlsx
+++ b/Examples/Dictionary/Input/Exp62_RatingsSetup_empty.xlsx
@@ -767,10 +767,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="8" t="n">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="D11" s="8" t="n">
-        <v>6.999999999999999</v>
+        <v>1</v>
       </c>
       <c r="E11" s="9" t="n"/>
       <c r="F11" s="10">
@@ -800,7 +800,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="9" t="n"/>
       <c r="F12" s="10">
@@ -1060,7 +1060,25 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <dataValidations count="12">
+    <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A5</formula1>
+    </dataValidation>
+    <dataValidation sqref="B3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A5</formula1>
+    </dataValidation>
+    <dataValidation sqref="B4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A5</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A11:A13</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A11:A13</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A11:A13</formula1>
+    </dataValidation>
     <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>=rating_scales!A3:A5</formula1>
     </dataValidation>

</xml_diff>